<commit_message>
ajout et correction sql
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://devinci-my.sharepoint.com/personal/aline_ellul_devinci_fr/Documents/Documents/CoursESILV2024/PSI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ECOLE\GITHUB\Projet_Livin-paris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{09A5E742-09C0-4DFC-88E0-A340CAFB2629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57D72C21-2BE2-4109-BDD7-01FB2A6C236E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34C1F22-8377-437C-8407-42285E00FF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A87F16E-6D3B-4C00-9BC9-6484A71C5A41}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6A87F16E-6D3B-4C00-9BC9-6484A71C5A41}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Numero</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Durand</t>
   </si>
   <si>
-    <t>Medhy</t>
-  </si>
-  <si>
     <t>Rue Cardinet</t>
   </si>
   <si>
@@ -84,6 +81,66 @@
   </si>
   <si>
     <t>Cardinet</t>
+  </si>
+  <si>
+    <t>Mathilde</t>
+  </si>
+  <si>
+    <t>Dorand</t>
+  </si>
+  <si>
+    <t>Darand</t>
+  </si>
+  <si>
+    <t>Dirand</t>
+  </si>
+  <si>
+    <t>Derand</t>
+  </si>
+  <si>
+    <t>Mothilde</t>
+  </si>
+  <si>
+    <t>Muthilde</t>
+  </si>
+  <si>
+    <t>Mithilde</t>
+  </si>
+  <si>
+    <t>Methilde</t>
+  </si>
+  <si>
+    <t>Rue Curdinet</t>
+  </si>
+  <si>
+    <t>Rue Cordinet</t>
+  </si>
+  <si>
+    <t>Rue Cirdinet</t>
+  </si>
+  <si>
+    <t>Rue Cerdinet</t>
+  </si>
+  <si>
+    <t>Mdorand@gmail.com</t>
+  </si>
+  <si>
+    <t>Mdarand@gmail.com</t>
+  </si>
+  <si>
+    <t>Mderand@gmail.com</t>
+  </si>
+  <si>
+    <t>Cordinet</t>
+  </si>
+  <si>
+    <t>Cirdinet</t>
+  </si>
+  <si>
+    <t>Cerdinet</t>
+  </si>
+  <si>
+    <t>Curdinet</t>
   </si>
 </sst>
 </file>
@@ -150,9 +207,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +247,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -296,7 +353,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -438,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEFA4ED-860A-4C8B-AAF2-7FCC00C1D146}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,7 +543,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -497,34 +554,166 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>75017</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>1234567890</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>75017</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>1234567899</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>75017</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>2345678901</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>75017</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>3456789012</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>75017</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>4567890123</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{FAEFA4ED-860A-4C8B-AAF2-7FCC00C1D146}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{443CDC48-7CB9-40F6-9739-F88F229D3F3D}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{AAE8B0FB-379F-469A-B9F1-B37FFAA5D192}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{C7419F8D-3A2D-4F98-85D3-C42838D225DE}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{D6DE5ABA-C0E4-4B95-8ADD-BC679BB551AF}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{D16A4C1E-363D-4BA0-B431-4CFC5F87E3B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>